<commit_message>
update albacore, remove duplicate Omy
</commit_message>
<xml_diff>
--- a/Panel_info/Ots28_marker_info.xlsx
+++ b/Panel_info/Ots28_marker_info.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ddayan/FRA/GT-Seq_SOP/GT-seq/Panel_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5DE58A-178B-9045-9039-41A2DF3FC9DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A3DA19-5415-0A4E-9ADB-C567000283C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{B4E73EBE-64E0-AE43-A1C0-CDF4588F1C5D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" activeTab="1" xr2:uid="{B4E73EBE-64E0-AE43-A1C0-CDF4588F1C5D}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="marker_info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
   <si>
     <t xml:space="preserve">Summary: </t>
   </si>
@@ -269,6 +269,15 @@
   </si>
   <si>
     <t>mapped position of SNP in probe sequence on Otsh_v1.0 (GCA_002872995.1) assembly, note: this information is from different sources, one of the files does not describe the reference genome used, so if we want to be confident in these values we should do our own mapping of amplicons</t>
+  </si>
+  <si>
+    <t>alternate ID3</t>
+  </si>
+  <si>
+    <t>Scaffold79929e:640165</t>
+  </si>
+  <si>
+    <t>Scaffold79929e:670329</t>
   </si>
 </sst>
 </file>
@@ -320,20 +329,20 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -692,65 +701,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D13" t="s">
@@ -758,20 +767,20 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>69</v>
       </c>
       <c r="D15" t="s">
@@ -779,7 +788,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
@@ -787,7 +796,7 @@
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
@@ -795,7 +804,7 @@
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
@@ -803,7 +812,7 @@
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
@@ -821,10 +830,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919FB259-8A00-4E43-816F-33DE21848C05}">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -832,42 +841,46 @@
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
@@ -883,15 +896,15 @@
         <f>D3-D2</f>
         <v>2068</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
@@ -907,15 +920,15 @@
         <f t="shared" ref="E3:E35" si="0">D4-D3</f>
         <v>8437</v>
       </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
@@ -931,15 +944,15 @@
         <f t="shared" si="0"/>
         <v>24496</v>
       </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
       <c r="I4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
@@ -955,15 +968,15 @@
         <f t="shared" si="0"/>
         <v>1389</v>
       </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B6" t="s">
@@ -985,16 +998,16 @@
       <c r="G6" t="s">
         <v>51</v>
       </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
       <c r="I6" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B7" t="s">
@@ -1016,18 +1029,18 @@
       <c r="G7" t="s">
         <v>56</v>
       </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
       <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
         <v>0</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B8" t="s">
@@ -1049,15 +1062,15 @@
       <c r="G8" t="s">
         <v>52</v>
       </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
       <c r="I8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
@@ -1073,15 +1086,15 @@
         <f t="shared" si="0"/>
         <v>598</v>
       </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
@@ -1097,15 +1110,15 @@
         <f t="shared" si="0"/>
         <v>1598</v>
       </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
@@ -1121,15 +1134,15 @@
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
       <c r="I11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
@@ -1145,15 +1158,15 @@
         <f t="shared" si="0"/>
         <v>443</v>
       </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
       <c r="I12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B13" t="s">
@@ -1175,15 +1188,18 @@
       <c r="G13" t="s">
         <v>53</v>
       </c>
-      <c r="H13" t="b">
-        <v>1</v>
+      <c r="H13" t="s">
+        <v>79</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
@@ -1199,15 +1215,15 @@
         <f t="shared" si="0"/>
         <v>1618</v>
       </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
       <c r="I14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B15" t="s">
@@ -1229,18 +1245,18 @@
       <c r="G15" t="s">
         <v>57</v>
       </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
@@ -1256,15 +1272,15 @@
         <f t="shared" si="0"/>
         <v>364</v>
       </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
       <c r="I16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
@@ -1280,15 +1296,15 @@
         <f t="shared" si="0"/>
         <v>1262</v>
       </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
       <c r="I17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
@@ -1304,15 +1320,15 @@
         <f t="shared" si="0"/>
         <v>194</v>
       </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
       <c r="I18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
@@ -1328,15 +1344,15 @@
         <f t="shared" si="0"/>
         <v>245</v>
       </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
       <c r="I19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B20" t="s">
@@ -1358,15 +1374,15 @@
       <c r="G20" t="s">
         <v>54</v>
       </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
       <c r="I20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" t="s">
@@ -1382,15 +1398,15 @@
         <f t="shared" si="0"/>
         <v>18484</v>
       </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
@@ -1406,15 +1422,15 @@
         <f t="shared" si="0"/>
         <v>10803</v>
       </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
       <c r="I22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B23" t="s">
@@ -1436,15 +1452,18 @@
       <c r="G23" t="s">
         <v>55</v>
       </c>
-      <c r="H23" t="b">
-        <v>1</v>
+      <c r="H23" t="s">
+        <v>80</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
@@ -1460,15 +1479,15 @@
         <f t="shared" si="0"/>
         <v>17681</v>
       </c>
-      <c r="H24" t="b">
-        <v>1</v>
-      </c>
       <c r="I24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
@@ -1484,15 +1503,15 @@
         <f t="shared" si="0"/>
         <v>3990</v>
       </c>
-      <c r="H25" t="b">
-        <v>1</v>
-      </c>
       <c r="I25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="J25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
@@ -1508,15 +1527,15 @@
         <f t="shared" si="0"/>
         <v>22707</v>
       </c>
-      <c r="H26" t="b">
-        <v>1</v>
-      </c>
       <c r="I26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B27" t="s">
@@ -1532,15 +1551,15 @@
         <f t="shared" si="0"/>
         <v>14540</v>
       </c>
-      <c r="H27" t="b">
-        <v>1</v>
-      </c>
       <c r="I27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B28" t="s">
@@ -1556,15 +1575,15 @@
         <f t="shared" si="0"/>
         <v>1061</v>
       </c>
-      <c r="H28" t="b">
-        <v>1</v>
-      </c>
       <c r="I28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B29" t="s">
@@ -1580,15 +1599,15 @@
         <f t="shared" si="0"/>
         <v>209</v>
       </c>
-      <c r="H29" t="b">
-        <v>1</v>
-      </c>
       <c r="I29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B30" t="s">
@@ -1604,15 +1623,15 @@
         <f t="shared" si="0"/>
         <v>464</v>
       </c>
-      <c r="H30" t="b">
-        <v>1</v>
-      </c>
       <c r="I30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
@@ -1628,15 +1647,15 @@
         <f t="shared" si="0"/>
         <v>2541</v>
       </c>
-      <c r="H31" t="b">
-        <v>1</v>
-      </c>
       <c r="I31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B32" t="s">
@@ -1652,15 +1671,15 @@
         <f t="shared" si="0"/>
         <v>564</v>
       </c>
-      <c r="H32" t="b">
-        <v>1</v>
-      </c>
       <c r="I32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B33" t="s">
@@ -1676,15 +1695,15 @@
         <f t="shared" si="0"/>
         <v>747</v>
       </c>
-      <c r="H33" t="b">
-        <v>1</v>
-      </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
@@ -1700,15 +1719,15 @@
         <f t="shared" si="0"/>
         <v>618</v>
       </c>
-      <c r="H34" t="b">
-        <v>1</v>
-      </c>
       <c r="I34" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
@@ -1724,15 +1743,15 @@
         <f t="shared" si="0"/>
         <v>3489</v>
       </c>
-      <c r="H35" t="b">
-        <v>1</v>
-      </c>
       <c r="I35" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="J35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B36" t="s">
@@ -1747,198 +1766,198 @@
       <c r="E36" t="s">
         <v>67</v>
       </c>
-      <c r="H36" t="b">
-        <v>1</v>
-      </c>
       <c r="I36" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
+      <c r="A49" s="1"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
+      <c r="A50" s="1"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
+      <c r="A51" s="1"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
+      <c r="A52" s="1"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
+      <c r="A53" s="1"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
+      <c r="A54" s="1"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
+      <c r="A55" s="2"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
+      <c r="A56" s="1"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
+      <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
+      <c r="A58" s="1"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
+      <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
+      <c r="A60" s="1"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
+      <c r="A61" s="1"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
+      <c r="A62" s="1"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
+      <c r="A63" s="1"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
+      <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
+      <c r="A65" s="1"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
+      <c r="A66" s="1"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
+      <c r="A67" s="1"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
+      <c r="A68" s="1"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="2"/>
+      <c r="A69" s="1"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="2"/>
+      <c r="A70" s="1"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="2"/>
+      <c r="A71" s="1"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="2"/>
+      <c r="A72" s="1"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="2"/>
+      <c r="A73" s="1"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="2"/>
+      <c r="A74" s="1"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="2"/>
+      <c r="A75" s="1"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="2"/>
+      <c r="A76" s="1"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="2"/>
+      <c r="A77" s="1"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="2"/>
+      <c r="A78" s="1"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="2"/>
+      <c r="A79" s="1"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="2"/>
+      <c r="A80" s="1"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="2"/>
+      <c r="A81" s="1"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="2"/>
+      <c r="A82" s="1"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="2"/>
+      <c r="A83" s="1"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="2"/>
+      <c r="A84" s="1"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="2"/>
+      <c r="A85" s="1"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="2"/>
+      <c r="A86" s="1"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="2"/>
+      <c r="A87" s="1"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="2"/>
+      <c r="A88" s="1"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="2"/>
+      <c r="A89" s="1"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="2"/>
+      <c r="A90" s="1"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="2"/>
+      <c r="A91" s="1"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" s="2"/>
+      <c r="A92" s="1"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="2"/>
+      <c r="A93" s="1"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="2"/>
+      <c r="A94" s="1"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95" s="2"/>
+      <c r="A95" s="1"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" s="2"/>
+      <c r="A96" s="1"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="2"/>
+      <c r="A97" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K36">
     <sortCondition ref="D2:D36"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1948,9 +1967,9 @@
   <conditionalFormatting sqref="A91:A97">
     <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:I36">
+  <conditionalFormatting sqref="I2:J36">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>